<commit_message>
pulled date range creation to it's own function
</commit_message>
<xml_diff>
--- a/personnel_sample.xlsx
+++ b/personnel_sample.xlsx
@@ -5,7 +5,8 @@
   <sheets>
     <sheet state="visible" name="settings" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="positions" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="inflation" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="related" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="inflation" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t>setting_name</t>
   </si>
@@ -115,6 +116,33 @@
   </si>
   <si>
     <t>Eve</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>expense_type</t>
+  </si>
+  <si>
+    <t>amount_annual</t>
+  </si>
+  <si>
+    <t>Stock compensation</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>Home office allowance</t>
+  </si>
+  <si>
+    <t>office expense</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>travel</t>
   </si>
   <si>
     <t>inflation_date</t>
@@ -127,8 +155,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -157,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -173,6 +202,9 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="14" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
@@ -193,6 +225,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -617,7 +653,7 @@
         <v>33</v>
       </c>
       <c r="F6" s="4">
-        <v>95000.0</v>
+        <v>100000.0</v>
       </c>
       <c r="G6" s="3">
         <v>0.1</v>
@@ -646,14 +682,157 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="1">
+        <v>10000.0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>44562.0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>45291.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1200.0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>44576.0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>44972.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5000.0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>44561.0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>44654.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <f>settings!B2</f>
         <v>44562</v>
       </c>
@@ -662,41 +841,41 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="7">
         <f t="shared" ref="A3:A6" si="1">EDATE(A2,12)</f>
         <v>44927</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="8">
         <f>B2*1.08</f>
         <v>1.08</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="7">
         <f t="shared" si="1"/>
         <v>45292</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="8">
         <f>B3*1.05</f>
         <v>1.134</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="7">
         <f t="shared" si="1"/>
         <v>45658</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="8">
         <f t="shared" ref="B5:B6" si="2">round(B4*1.03,3)</f>
         <v>1.168</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="7">
         <f t="shared" si="1"/>
         <v>46023</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="8">
         <f t="shared" si="2"/>
         <v>1.203</v>
       </c>

</xml_diff>

<commit_message>
Added inputs for recurring and one time personnel related expenses and updated forecast to include these
</commit_message>
<xml_diff>
--- a/personnel_sample.xlsx
+++ b/personnel_sample.xlsx
@@ -6,7 +6,8 @@
     <sheet state="visible" name="settings" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="positions" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="related" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="inflation" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="onetime" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="inflation" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
   <si>
     <t>setting_name</t>
   </si>
@@ -143,6 +144,18 @@
   </si>
   <si>
     <t>travel</t>
+  </si>
+  <si>
+    <t>expense_amount</t>
+  </si>
+  <si>
+    <t>expense_date</t>
+  </si>
+  <si>
+    <t>signing bonud</t>
+  </si>
+  <si>
+    <t>severance</t>
   </si>
   <si>
     <t>inflation_date</t>
@@ -229,6 +242,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -600,9 +617,7 @@
       <c r="H4" s="3">
         <v>0.0</v>
       </c>
-      <c r="I4" s="2">
-        <v>44561.0</v>
-      </c>
+      <c r="I4" s="2"/>
       <c r="J4" s="2">
         <v>44654.0</v>
       </c>
@@ -634,6 +649,9 @@
       </c>
       <c r="I5" s="2">
         <v>44561.0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>44727.0</v>
       </c>
     </row>
     <row r="6">
@@ -825,10 +843,115 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="4">
+        <v>10000.0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>44607.0</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="4">
+        <v>5000.0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>44727.0</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="5"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2">

</xml_diff>